<commit_message>
Generate Salary Formula fields
</commit_message>
<xml_diff>
--- a/documents/employees/EMPLOYEES.xlsx
+++ b/documents/employees/EMPLOYEES.xlsx
@@ -1569,12 +1569,42 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1582,36 +1612,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2429,8 +2429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AM2" sqref="AM2"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4344,46 +4344,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="12" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="159" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
-      <c r="D1" s="151"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="161"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="152"/>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="154"/>
+      <c r="A2" s="155"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="157"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="155"/>
-      <c r="B3" s="156"/>
-      <c r="C3" s="156"/>
-      <c r="D3" s="157"/>
+      <c r="A3" s="158"/>
+      <c r="B3" s="148"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="149"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="155"/>
-      <c r="B4" s="156"/>
-      <c r="C4" s="156"/>
-      <c r="D4" s="157"/>
+      <c r="A4" s="158"/>
+      <c r="B4" s="148"/>
+      <c r="C4" s="148"/>
+      <c r="D4" s="149"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="158" t="s">
+      <c r="A5" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="159"/>
-      <c r="C5" s="159"/>
-      <c r="D5" s="160"/>
+      <c r="B5" s="153"/>
+      <c r="C5" s="153"/>
+      <c r="D5" s="154"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="161" t="s">
+      <c r="A6" s="147" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="156"/>
-      <c r="C6" s="156"/>
-      <c r="D6" s="157"/>
+      <c r="B6" s="148"/>
+      <c r="C6" s="148"/>
+      <c r="D6" s="149"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="14" t="s">
@@ -4505,47 +4505,47 @@
       <c r="A18" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="147">
+      <c r="B18" s="150">
         <f>B17-D17</f>
         <v>0</v>
       </c>
-      <c r="C18" s="147"/>
-      <c r="D18" s="148"/>
+      <c r="C18" s="150"/>
+      <c r="D18" s="151"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="21" spans="1:4">
-      <c r="A21" s="152"/>
-      <c r="B21" s="153"/>
-      <c r="C21" s="153"/>
-      <c r="D21" s="154"/>
+      <c r="A21" s="155"/>
+      <c r="B21" s="156"/>
+      <c r="C21" s="156"/>
+      <c r="D21" s="157"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="155"/>
-      <c r="B22" s="156"/>
-      <c r="C22" s="156"/>
-      <c r="D22" s="157"/>
+      <c r="A22" s="158"/>
+      <c r="B22" s="148"/>
+      <c r="C22" s="148"/>
+      <c r="D22" s="149"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="155"/>
-      <c r="B23" s="156"/>
-      <c r="C23" s="156"/>
-      <c r="D23" s="157"/>
+      <c r="A23" s="158"/>
+      <c r="B23" s="148"/>
+      <c r="C23" s="148"/>
+      <c r="D23" s="149"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="158" t="s">
+      <c r="A24" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="B24" s="159"/>
-      <c r="C24" s="159"/>
-      <c r="D24" s="160"/>
+      <c r="B24" s="153"/>
+      <c r="C24" s="153"/>
+      <c r="D24" s="154"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="161" t="s">
+      <c r="A25" s="147" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="156"/>
-      <c r="C25" s="156"/>
-      <c r="D25" s="157"/>
+      <c r="B25" s="148"/>
+      <c r="C25" s="148"/>
+      <c r="D25" s="149"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="14" t="s">
@@ -4667,47 +4667,47 @@
       <c r="A37" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="147">
+      <c r="B37" s="150">
         <f>B36-D36</f>
         <v>0</v>
       </c>
-      <c r="C37" s="147"/>
-      <c r="D37" s="148"/>
+      <c r="C37" s="150"/>
+      <c r="D37" s="151"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="40" spans="1:4">
-      <c r="A40" s="152"/>
-      <c r="B40" s="153"/>
-      <c r="C40" s="153"/>
-      <c r="D40" s="154"/>
+      <c r="A40" s="155"/>
+      <c r="B40" s="156"/>
+      <c r="C40" s="156"/>
+      <c r="D40" s="157"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="155"/>
-      <c r="B41" s="156"/>
-      <c r="C41" s="156"/>
-      <c r="D41" s="157"/>
+      <c r="A41" s="158"/>
+      <c r="B41" s="148"/>
+      <c r="C41" s="148"/>
+      <c r="D41" s="149"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="155"/>
-      <c r="B42" s="156"/>
-      <c r="C42" s="156"/>
-      <c r="D42" s="157"/>
+      <c r="A42" s="158"/>
+      <c r="B42" s="148"/>
+      <c r="C42" s="148"/>
+      <c r="D42" s="149"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="158" t="s">
+      <c r="A43" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="B43" s="159"/>
-      <c r="C43" s="159"/>
-      <c r="D43" s="160"/>
+      <c r="B43" s="153"/>
+      <c r="C43" s="153"/>
+      <c r="D43" s="154"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="161" t="s">
+      <c r="A44" s="147" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="156"/>
-      <c r="C44" s="156"/>
-      <c r="D44" s="157"/>
+      <c r="B44" s="148"/>
+      <c r="C44" s="148"/>
+      <c r="D44" s="149"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="14" t="s">
@@ -4829,47 +4829,47 @@
       <c r="A56" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B56" s="147">
+      <c r="B56" s="150">
         <f>B55-D55</f>
         <v>0</v>
       </c>
-      <c r="C56" s="147"/>
-      <c r="D56" s="148"/>
+      <c r="C56" s="150"/>
+      <c r="D56" s="151"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="59" spans="1:4">
-      <c r="A59" s="152"/>
-      <c r="B59" s="153"/>
-      <c r="C59" s="153"/>
-      <c r="D59" s="154"/>
+      <c r="A59" s="155"/>
+      <c r="B59" s="156"/>
+      <c r="C59" s="156"/>
+      <c r="D59" s="157"/>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="155"/>
-      <c r="B60" s="156"/>
-      <c r="C60" s="156"/>
-      <c r="D60" s="157"/>
+      <c r="A60" s="158"/>
+      <c r="B60" s="148"/>
+      <c r="C60" s="148"/>
+      <c r="D60" s="149"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="155"/>
-      <c r="B61" s="156"/>
-      <c r="C61" s="156"/>
-      <c r="D61" s="157"/>
+      <c r="A61" s="158"/>
+      <c r="B61" s="148"/>
+      <c r="C61" s="148"/>
+      <c r="D61" s="149"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="158" t="s">
+      <c r="A62" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="B62" s="159"/>
-      <c r="C62" s="159"/>
-      <c r="D62" s="160"/>
+      <c r="B62" s="153"/>
+      <c r="C62" s="153"/>
+      <c r="D62" s="154"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="161" t="s">
+      <c r="A63" s="147" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="156"/>
-      <c r="C63" s="156"/>
-      <c r="D63" s="157"/>
+      <c r="B63" s="148"/>
+      <c r="C63" s="148"/>
+      <c r="D63" s="149"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="14" t="s">
@@ -4991,47 +4991,47 @@
       <c r="A75" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B75" s="147">
+      <c r="B75" s="150">
         <f>B74-D74</f>
         <v>0</v>
       </c>
-      <c r="C75" s="147"/>
-      <c r="D75" s="148"/>
+      <c r="C75" s="150"/>
+      <c r="D75" s="151"/>
     </row>
     <row r="77" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="78" spans="1:4">
-      <c r="A78" s="152"/>
-      <c r="B78" s="153"/>
-      <c r="C78" s="153"/>
-      <c r="D78" s="154"/>
+      <c r="A78" s="155"/>
+      <c r="B78" s="156"/>
+      <c r="C78" s="156"/>
+      <c r="D78" s="157"/>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="155"/>
-      <c r="B79" s="156"/>
-      <c r="C79" s="156"/>
-      <c r="D79" s="157"/>
+      <c r="A79" s="158"/>
+      <c r="B79" s="148"/>
+      <c r="C79" s="148"/>
+      <c r="D79" s="149"/>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="155"/>
-      <c r="B80" s="156"/>
-      <c r="C80" s="156"/>
-      <c r="D80" s="157"/>
+      <c r="A80" s="158"/>
+      <c r="B80" s="148"/>
+      <c r="C80" s="148"/>
+      <c r="D80" s="149"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="158" t="s">
+      <c r="A81" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="B81" s="159"/>
-      <c r="C81" s="159"/>
-      <c r="D81" s="160"/>
+      <c r="B81" s="153"/>
+      <c r="C81" s="153"/>
+      <c r="D81" s="154"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="161" t="s">
+      <c r="A82" s="147" t="s">
         <v>62</v>
       </c>
-      <c r="B82" s="156"/>
-      <c r="C82" s="156"/>
-      <c r="D82" s="157"/>
+      <c r="B82" s="148"/>
+      <c r="C82" s="148"/>
+      <c r="D82" s="149"/>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="14" t="s">
@@ -5153,47 +5153,47 @@
       <c r="A94" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B94" s="147">
+      <c r="B94" s="150">
         <f>B93-D93</f>
         <v>0</v>
       </c>
-      <c r="C94" s="147"/>
-      <c r="D94" s="148"/>
+      <c r="C94" s="150"/>
+      <c r="D94" s="151"/>
     </row>
     <row r="96" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="97" spans="1:4">
-      <c r="A97" s="152"/>
-      <c r="B97" s="153"/>
-      <c r="C97" s="153"/>
-      <c r="D97" s="154"/>
+      <c r="A97" s="155"/>
+      <c r="B97" s="156"/>
+      <c r="C97" s="156"/>
+      <c r="D97" s="157"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="155"/>
-      <c r="B98" s="156"/>
-      <c r="C98" s="156"/>
-      <c r="D98" s="157"/>
+      <c r="A98" s="158"/>
+      <c r="B98" s="148"/>
+      <c r="C98" s="148"/>
+      <c r="D98" s="149"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="155"/>
-      <c r="B99" s="156"/>
-      <c r="C99" s="156"/>
-      <c r="D99" s="157"/>
+      <c r="A99" s="158"/>
+      <c r="B99" s="148"/>
+      <c r="C99" s="148"/>
+      <c r="D99" s="149"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="158" t="s">
+      <c r="A100" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="B100" s="159"/>
-      <c r="C100" s="159"/>
-      <c r="D100" s="160"/>
+      <c r="B100" s="153"/>
+      <c r="C100" s="153"/>
+      <c r="D100" s="154"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="161" t="s">
+      <c r="A101" s="147" t="s">
         <v>62</v>
       </c>
-      <c r="B101" s="156"/>
-      <c r="C101" s="156"/>
-      <c r="D101" s="157"/>
+      <c r="B101" s="148"/>
+      <c r="C101" s="148"/>
+      <c r="D101" s="149"/>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="14" t="s">
@@ -5315,47 +5315,47 @@
       <c r="A113" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B113" s="147">
+      <c r="B113" s="150">
         <f>B112-D112</f>
         <v>0</v>
       </c>
-      <c r="C113" s="147"/>
-      <c r="D113" s="148"/>
+      <c r="C113" s="150"/>
+      <c r="D113" s="151"/>
     </row>
     <row r="115" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="116" spans="1:4">
-      <c r="A116" s="152"/>
-      <c r="B116" s="153"/>
-      <c r="C116" s="153"/>
-      <c r="D116" s="154"/>
+      <c r="A116" s="155"/>
+      <c r="B116" s="156"/>
+      <c r="C116" s="156"/>
+      <c r="D116" s="157"/>
     </row>
     <row r="117" spans="1:4">
-      <c r="A117" s="155"/>
-      <c r="B117" s="156"/>
-      <c r="C117" s="156"/>
-      <c r="D117" s="157"/>
+      <c r="A117" s="158"/>
+      <c r="B117" s="148"/>
+      <c r="C117" s="148"/>
+      <c r="D117" s="149"/>
     </row>
     <row r="118" spans="1:4">
-      <c r="A118" s="155"/>
-      <c r="B118" s="156"/>
-      <c r="C118" s="156"/>
-      <c r="D118" s="157"/>
+      <c r="A118" s="158"/>
+      <c r="B118" s="148"/>
+      <c r="C118" s="148"/>
+      <c r="D118" s="149"/>
     </row>
     <row r="119" spans="1:4">
-      <c r="A119" s="158" t="s">
+      <c r="A119" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="B119" s="159"/>
-      <c r="C119" s="159"/>
-      <c r="D119" s="160"/>
+      <c r="B119" s="153"/>
+      <c r="C119" s="153"/>
+      <c r="D119" s="154"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="161" t="s">
+      <c r="A120" s="147" t="s">
         <v>62</v>
       </c>
-      <c r="B120" s="156"/>
-      <c r="C120" s="156"/>
-      <c r="D120" s="157"/>
+      <c r="B120" s="148"/>
+      <c r="C120" s="148"/>
+      <c r="D120" s="149"/>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="14" t="s">
@@ -5477,42 +5477,15 @@
       <c r="A132" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B132" s="147">
+      <c r="B132" s="150">
         <f>B131-D131</f>
         <v>0</v>
       </c>
-      <c r="C132" s="147"/>
-      <c r="D132" s="148"/>
+      <c r="C132" s="150"/>
+      <c r="D132" s="151"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="B94:D94"/>
-    <mergeCell ref="A100:D100"/>
-    <mergeCell ref="A101:D101"/>
-    <mergeCell ref="B113:D113"/>
-    <mergeCell ref="A97:D97"/>
-    <mergeCell ref="A98:D98"/>
-    <mergeCell ref="A99:D99"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
     <mergeCell ref="B132:D132"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A116:D116"/>
@@ -5529,6 +5502,33 @@
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="A59:D59"/>
     <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="A100:D100"/>
+    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="B113:D113"/>
+    <mergeCell ref="A97:D97"/>
+    <mergeCell ref="A98:D98"/>
+    <mergeCell ref="A99:D99"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>